<commit_message>
Calculate Adj Net Income and add to dcf_inputs
</commit_message>
<xml_diff>
--- a/FLDCF20211006.xlsx
+++ b/FLDCF20211006.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhess/Library/Mobile Documents/com~apple~CloudDocs/Documents/Investing/Foot Locker/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6409ACE6-DDA4-6B4D-96EF-C0F054186E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B092176-A0C5-A743-8D7A-874001505211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="46200" yWindow="5680" windowWidth="27640" windowHeight="16940" xr2:uid="{D04705D2-C07A-DB40-90D7-A31F9015E733}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Income Statement" sheetId="2" r:id="rId3"/>
     <sheet name="Cash Flow Statement" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateDelta="9.9999999999994451E-4" concurrentCalc="0"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,9 +45,6 @@
     <t>Cash and Marketable Securities</t>
   </si>
   <si>
-    <t>Number of Shares Outstanding</t>
-  </si>
-  <si>
     <t>Current Assets</t>
   </si>
   <si>
@@ -66,18 +63,12 @@
     <t>High Growth Period in Years</t>
   </si>
   <si>
-    <t>Growth Rate for Stable Growth Period</t>
-  </si>
-  <si>
     <t>Stable Period Beta</t>
   </si>
   <si>
     <t>Net Income</t>
   </si>
   <si>
-    <t>Interest Income from Cash and Marketable Securities</t>
-  </si>
-  <si>
     <t>Current Depreciation</t>
   </si>
   <si>
@@ -102,16 +93,25 @@
     <t>CAPEX</t>
   </si>
   <si>
-    <t>Depreciation Amortization</t>
-  </si>
-  <si>
-    <t>Net Issuance Payments of debt</t>
-  </si>
-  <si>
-    <t>Net Common Stock Issuance</t>
-  </si>
-  <si>
     <t>Current Year</t>
+  </si>
+  <si>
+    <t>Interest Income</t>
+  </si>
+  <si>
+    <t>Shares Outstanding</t>
+  </si>
+  <si>
+    <t>Depreciation</t>
+  </si>
+  <si>
+    <t>Net New Debt</t>
+  </si>
+  <si>
+    <t>Net Stock Issuance</t>
+  </si>
+  <si>
+    <t>Stable Period Growth Rate</t>
   </si>
 </sst>
 </file>
@@ -482,7 +482,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -493,18 +493,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1">
         <v>4709</v>
@@ -515,7 +515,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1">
         <f>3189000/2771000</f>
@@ -524,7 +524,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1">
         <v>1.4</v>
@@ -532,7 +532,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
         <v>4.84</v>
@@ -540,7 +540,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
@@ -548,7 +548,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1">
         <v>4</v>
@@ -556,7 +556,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1">
         <v>1.1000000000000001</v>
@@ -621,7 +621,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -633,10 +633,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.25">
@@ -663,7 +663,7 @@
     </row>
     <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1">
         <v>103619</v>
@@ -671,7 +671,7 @@
     </row>
     <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1">
         <v>2835000</v>
@@ -682,7 +682,7 @@
     </row>
     <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1">
         <v>1644000</v>
@@ -693,7 +693,7 @@
     </row>
     <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1">
         <v>3189000</v>
@@ -701,7 +701,7 @@
     </row>
     <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1">
         <v>2771000</v>
@@ -717,7 +717,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -728,15 +728,15 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1">
         <v>1020000</v>
@@ -744,7 +744,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1">
         <v>4000</v>
@@ -752,7 +752,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1">
         <v>181000</v>
@@ -768,7 +768,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -779,15 +779,15 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1">
         <v>1020000</v>
@@ -803,7 +803,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1">
         <v>-163000</v>

</xml_diff>